<commit_message>
data analysis. learning pandas, matplotlib. some folder changes
</commit_message>
<xml_diff>
--- a/projects/covid/CoVid_data.xlsx
+++ b/projects/covid/CoVid_data.xlsx
@@ -12073,7 +12073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R88"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
@@ -16998,8 +16998,6 @@
           <t>14.7</t>
         </is>
       </c>
-      <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -17052,8 +17050,322 @@
           <t>15.2</t>
         </is>
       </c>
-      <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>13.04.2020</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1,923,848</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>+71,591</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>119,618</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>+5,423</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>444,636</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>1,359,594</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>51,747</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>246.8</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>15.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>14.04.2020</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>1,934,125</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>+10,277</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>120,437</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>+819</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>456,589</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>1,357,099</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>51,142</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>248.1</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>15.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>15.04.2020</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2,086,431</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>+84,796</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>138,619</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>+8,241</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>510,046</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>1,437,766</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>51,160</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>267.7</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>17.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>16.04.2020</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2,115,624</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>+29,193</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>141,195</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>+2,576</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>527,471</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>1,446,958</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>51,108</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>271.4</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>18.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>16.04.2020</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2,181,308</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>+95,022</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>145,470</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>+6,996</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>547,069</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>1,488,769</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>56,602</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>279.8</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>18.7</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>17.04.2020</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2,182,823</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>+1,515</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>145,551</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>+81</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>547,679</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>1,489,593</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>56,588</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>280.0</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>18.7</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
covid analysis. start us_names analysis
</commit_message>
<xml_diff>
--- a/projects/covid/CoVid_data.xlsx
+++ b/projects/covid/CoVid_data.xlsx
@@ -12073,7 +12073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
@@ -17310,8 +17310,6 @@
           <t>18.7</t>
         </is>
       </c>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -17364,8 +17362,114 @@
           <t>18.7</t>
         </is>
       </c>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>18.04.2020</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2,330,793</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>+81,930</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>160,643</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>+6,505</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>596,482</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>1,573,668</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>55,265</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>299.0</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>20.6</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>19.04.2020</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2,343,272</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>+12,479</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>161,190</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>+547</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>601,837</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>1,580,245</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>55,215</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>300.6</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>20.7</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
study matplotlib and diff graphs
</commit_message>
<xml_diff>
--- a/projects/covid/CoVid_data.xlsx
+++ b/projects/covid/CoVid_data.xlsx
@@ -12073,7 +12073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R96"/>
+  <dimension ref="A1:R98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
@@ -17414,8 +17414,6 @@
           <t>20.6</t>
         </is>
       </c>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -17468,8 +17466,114 @@
           <t>20.7</t>
         </is>
       </c>
-      <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>25.04.2020</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2,919,404</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>+90,722</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>203,164</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>+6,069</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>836,612</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>1,879,628</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>58,202</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>374.5</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>26.1</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>26.04.2020</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2,938,729</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>+19,325</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>203,798</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>+634</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>841,515</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>1,893,416</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>57,674</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>377.0</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>26.1</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr"/>
+      <c r="L98" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>